<commit_message>
Replaced and added new files and folders
</commit_message>
<xml_diff>
--- a/public/files/fs_livelihoods_economic/Vault_Sectors Individual.xlsx
+++ b/public/files/fs_livelihoods_economic/Vault_Sectors Individual.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UNHCR\Dropbox\VASYR 2019 Core Group\7_Data Tabulations\4_VASyR_VAULT\Food security\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stupalov\Dropbox\VASYR 2019 Core Group\7_Data Tabulations\4_VASyR_VAULT\FS_Livelihoods_Economic_DONE\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="METAData" sheetId="3" r:id="rId1"/>
@@ -785,6 +785,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -812,16 +813,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1149,8 +1149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1375,7 +1375,7 @@
       <c r="C13" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D13" s="56" t="s">
+      <c r="D13" s="44" t="s">
         <v>92</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -1392,7 +1392,7 @@
       <c r="C14" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="56" t="s">
+      <c r="D14" s="44" t="s">
         <v>93</v>
       </c>
       <c r="E14" s="4" t="s">
@@ -1409,7 +1409,7 @@
       <c r="C15" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="56" t="s">
+      <c r="D15" s="44" t="s">
         <v>94</v>
       </c>
       <c r="E15" s="4" t="s">
@@ -1426,7 +1426,7 @@
       <c r="C16" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="D16" s="56" t="s">
+      <c r="D16" s="44" t="s">
         <v>95</v>
       </c>
       <c r="E16" s="4" t="s">
@@ -1448,8 +1448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z65"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1494,47 +1494,47 @@
       <c r="Z1" s="10"/>
     </row>
     <row r="2" spans="1:26" s="18" customFormat="1" ht="47.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="47"/>
-      <c r="B2" s="44" t="s">
+      <c r="A2" s="48"/>
+      <c r="B2" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="49" t="s">
+      <c r="C2" s="45"/>
+      <c r="D2" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="50"/>
-      <c r="F2" s="51" t="s">
+      <c r="E2" s="51"/>
+      <c r="F2" s="52" t="s">
         <v>45</v>
       </c>
-      <c r="G2" s="52"/>
-      <c r="H2" s="53" t="s">
+      <c r="G2" s="53"/>
+      <c r="H2" s="55" t="s">
         <v>46</v>
       </c>
-      <c r="I2" s="54"/>
-      <c r="J2" s="55" t="s">
+      <c r="I2" s="56"/>
+      <c r="J2" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="K2" s="46"/>
-      <c r="L2" s="44" t="s">
+      <c r="K2" s="47"/>
+      <c r="L2" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="M2" s="44"/>
+      <c r="M2" s="45"/>
       <c r="N2" s="12" t="s">
         <v>49</v>
       </c>
       <c r="O2" s="13"/>
-      <c r="P2" s="45" t="s">
+      <c r="P2" s="46" t="s">
         <v>50</v>
       </c>
-      <c r="Q2" s="46"/>
-      <c r="R2" s="45" t="s">
+      <c r="Q2" s="47"/>
+      <c r="R2" s="46" t="s">
         <v>51</v>
       </c>
-      <c r="S2" s="46"/>
-      <c r="T2" s="45" t="s">
+      <c r="S2" s="47"/>
+      <c r="T2" s="46" t="s">
         <v>52</v>
       </c>
-      <c r="U2" s="46"/>
+      <c r="U2" s="47"/>
       <c r="V2" s="14" t="s">
         <v>53</v>
       </c>
@@ -1552,7 +1552,7 @@
       </c>
     </row>
     <row r="3" spans="1:26" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="48"/>
+      <c r="A3" s="49"/>
       <c r="B3" s="19" t="s">
         <v>40</v>
       </c>

</xml_diff>